<commit_message>
[Update] file Bugs list
</commit_message>
<xml_diff>
--- a/TOEIC-PREP-DATA - Bugs list.xlsx
+++ b/TOEIC-PREP-DATA - Bugs list.xlsx
@@ -9,20 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9060" tabRatio="920" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9060" tabRatio="920"/>
   </bookViews>
   <sheets>
     <sheet name="Defect List" sheetId="2" r:id="rId1"/>
-    <sheet name="Test Evidence #4" sheetId="8" r:id="rId2"/>
-    <sheet name="Test Evidence #5" sheetId="9" r:id="rId3"/>
-    <sheet name="Test Evidence #6" sheetId="10" r:id="rId4"/>
-    <sheet name="Test Evidence #7" sheetId="11" r:id="rId5"/>
-    <sheet name="Test Evidence #8" sheetId="12" r:id="rId6"/>
-    <sheet name="Test Evidence #9" sheetId="13" r:id="rId7"/>
-    <sheet name="Test Evidence #10" sheetId="14" r:id="rId8"/>
-    <sheet name="Test Evidence #1" sheetId="3" r:id="rId9"/>
-    <sheet name="Test evidence #2" sheetId="4" r:id="rId10"/>
-    <sheet name="Test Evidence #3" sheetId="5" r:id="rId11"/>
+    <sheet name="Test Evidence #1" sheetId="3" r:id="rId2"/>
+    <sheet name="Test evidence #2" sheetId="4" r:id="rId3"/>
+    <sheet name="Test Evidence #3" sheetId="5" r:id="rId4"/>
+    <sheet name="Test Evidence #4" sheetId="8" r:id="rId5"/>
+    <sheet name="Test Evidence #5" sheetId="9" r:id="rId6"/>
+    <sheet name="Test Evidence #6" sheetId="10" r:id="rId7"/>
+    <sheet name="Test Evidence #7" sheetId="11" r:id="rId8"/>
+    <sheet name="Test Evidence #8" sheetId="12" r:id="rId9"/>
+    <sheet name="Test Evidence #9" sheetId="13" r:id="rId10"/>
+    <sheet name="Test Evidence #10" sheetId="14" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
   <si>
     <t>Environment</t>
   </si>
@@ -405,7 +405,10 @@
     <t>Nhập dữ liệu thiếu đáp án ở cột A</t>
   </si>
   <si>
-    <t xml:space="preserve">Web đang lỗi hẹn gặp lại sau :3 </t>
+    <t>Nhập dữ liệu đầu vào</t>
+  </si>
+  <si>
+    <t>Send password tới mail</t>
   </si>
 </sst>
 </file>
@@ -680,6 +683,368 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>28309</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>170619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="598714" y="571500"/>
+          <a:ext cx="13009524" cy="6647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>28309</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>180143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="598714" y="7810500"/>
+          <a:ext cx="13009524" cy="6657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>28309</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>170619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="598714" y="15049500"/>
+          <a:ext cx="13009524" cy="6647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>569874</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>161095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="571500"/>
+          <a:ext cx="13009524" cy="6638095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>569874</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>180143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="7810500"/>
+          <a:ext cx="13009524" cy="6657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>274599</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>170619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="600075" y="571500"/>
+          <a:ext cx="13009524" cy="6647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>274599</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>170619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="600075" y="7810500"/>
+          <a:ext cx="13009524" cy="6647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>93624</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>170619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="571500"/>
+          <a:ext cx="13009524" cy="6647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>93624</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>170619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="7810500"/>
+          <a:ext cx="13009524" cy="6647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
@@ -794,7 +1159,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -913,7 +1278,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -994,7 +1359,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1075,7 +1440,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1156,7 +1521,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1188,87 +1553,6 @@
         <a:xfrm>
           <a:off x="609600" y="571500"/>
           <a:ext cx="13009524" cy="6647619"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>569874</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>161095</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="571500"/>
-          <a:ext cx="13009524" cy="6638095"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>569874</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>180143</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="7810500"/>
-          <a:ext cx="13009524" cy="6657143"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1569,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2082,55 +2366,169 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B79"/>
+  <dimension ref="B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="1"/>
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2"/>
+  <dimension ref="B2:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B79"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="B78" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B79"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:B40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
@@ -2160,7 +2558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B78"/>
   <sheetViews>
@@ -2194,7 +2592,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B35"/>
   <sheetViews>
@@ -2223,7 +2621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B34"/>
   <sheetViews>
@@ -2252,7 +2650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B34"/>
   <sheetViews>
@@ -2279,89 +2677,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:2">
-      <c r="B2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B40"/>
-  <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:2">
-      <c r="B2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B79"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1"/>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[Update] test plan, bug list, test case, test design
</commit_message>
<xml_diff>
--- a/TOEIC-PREP-DATA - Bugs list.xlsx
+++ b/TOEIC-PREP-DATA - Bugs list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnNgo\Documents\GitHub\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anngo\Documents\GitHub\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -42,7 +42,7 @@
     <author>Tran Thi Lanh</author>
   </authors>
   <commentList>
-    <comment ref="E6" authorId="0" shapeId="0">
+    <comment ref="E7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0">
+    <comment ref="F7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
   <si>
     <t>Environment</t>
   </si>
@@ -410,6 +410,12 @@
   <si>
     <t>Send password tới mail</t>
   </si>
+  <si>
+    <t>Version website</t>
+  </si>
+  <si>
+    <t>xLMS 19.3</t>
+  </si>
 </sst>
 </file>
 
@@ -418,12 +424,26 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -604,14 +624,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -619,48 +639,50 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1851,10 +1873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1873,7 +1895,7 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="21"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -1914,449 +1936,461 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="45.75" customHeight="1">
-      <c r="A5" s="1"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A6" s="10" t="s">
+    <row r="5" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="45.75" customHeight="1">
+      <c r="A6" s="1"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="19.5" customHeight="1">
-      <c r="A7" s="21" t="s">
+    <row r="8" spans="1:7" ht="19.5" customHeight="1">
+      <c r="A8" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="25"/>
-    </row>
-    <row r="8" spans="1:7" ht="30">
-      <c r="A8" s="19" t="s">
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
+    </row>
+    <row r="9" spans="1:7" ht="30">
+      <c r="A9" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B9" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="15"/>
-    </row>
-    <row r="9" spans="1:7" ht="67.900000000000006" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14" t="s">
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:7" ht="81.75" customHeight="1">
+      <c r="A10" s="13"/>
+      <c r="B10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D10" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G10" s="16">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30">
-      <c r="A10" s="11" t="s">
+    <row r="11" spans="1:7" ht="30">
+      <c r="A11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B11" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="15"/>
-    </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="139.9" customHeight="1">
-      <c r="A11" s="13"/>
-      <c r="B11" s="17" t="s">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="139.9" customHeight="1">
+      <c r="A12" s="13"/>
+      <c r="B12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C12" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D12" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="16">
+      <c r="G12" s="16">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
-      <c r="A12" s="19" t="s">
+    <row r="13" spans="1:7" ht="30">
+      <c r="A13" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B13" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="15"/>
-    </row>
-    <row r="13" spans="1:7" ht="90">
-      <c r="A13" s="13"/>
-      <c r="B13" s="17" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:7" ht="90">
+      <c r="A14" s="13"/>
+      <c r="B14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C14" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D14" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G14" s="16">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="21">
-      <c r="A14" s="21" t="s">
+    <row r="15" spans="1:7" ht="21">
+      <c r="A15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="25"/>
-    </row>
-    <row r="15" spans="1:7" ht="30">
-      <c r="A15" s="19" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="26"/>
+    </row>
+    <row r="16" spans="1:7" ht="30">
+      <c r="A16" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B16" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="15"/>
-    </row>
-    <row r="16" spans="1:7" ht="105">
-      <c r="A16" s="13"/>
-      <c r="B16" s="17" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:7" ht="105">
+      <c r="A17" s="13"/>
+      <c r="B17" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C17" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D17" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G17" s="16">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30">
-      <c r="A17" s="19" t="s">
+    <row r="18" spans="1:7" ht="30">
+      <c r="A18" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B18" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="15"/>
-    </row>
-    <row r="18" spans="1:7" ht="120">
-      <c r="A18" s="13"/>
-      <c r="B18" s="17" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="1:7" ht="120">
+      <c r="A19" s="13"/>
+      <c r="B19" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C19" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D19" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G19" s="16">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="21">
-      <c r="A19" s="21" t="s">
+    <row r="20" spans="1:7" ht="21">
+      <c r="A20" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="1:7" ht="45">
-      <c r="A20" s="19" t="s">
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26"/>
+    </row>
+    <row r="21" spans="1:7" ht="45">
+      <c r="A21" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B21" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="15"/>
-    </row>
-    <row r="21" spans="1:7" ht="240">
-      <c r="A21" s="13"/>
-      <c r="B21" s="17" t="s">
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="1:7" ht="240">
+      <c r="A22" s="13"/>
+      <c r="B22" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C22" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D22" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E22" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F22" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="16">
+      <c r="G22" s="16">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45">
-      <c r="A22" s="19" t="s">
+    <row r="23" spans="1:7" ht="45">
+      <c r="A23" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B23" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="15"/>
-    </row>
-    <row r="23" spans="1:7" ht="270">
-      <c r="A23" s="13"/>
-      <c r="B23" s="17" t="s">
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="15"/>
+    </row>
+    <row r="24" spans="1:7" ht="270">
+      <c r="A24" s="13"/>
+      <c r="B24" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C24" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D24" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E24" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F24" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="16">
+      <c r="G24" s="16">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="45">
-      <c r="A24" s="19" t="s">
+    <row r="25" spans="1:7" ht="45">
+      <c r="A25" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B25" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="15"/>
-    </row>
-    <row r="25" spans="1:7" ht="270">
-      <c r="A25" s="13"/>
-      <c r="B25" s="17" t="s">
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="15"/>
+    </row>
+    <row r="26" spans="1:7" ht="270">
+      <c r="A26" s="13"/>
+      <c r="B26" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C26" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D26" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E26" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F26" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="16">
+      <c r="G26" s="16">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="21">
-      <c r="A26" s="21" t="s">
+    <row r="27" spans="1:7" ht="21">
+      <c r="A27" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="25"/>
-    </row>
-    <row r="27" spans="1:7" ht="30">
-      <c r="A27" s="19" t="s">
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="26"/>
+    </row>
+    <row r="28" spans="1:7" ht="30">
+      <c r="A28" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B28" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="1:7" ht="105">
-      <c r="A28" s="13"/>
-      <c r="B28" s="17" t="s">
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="15"/>
+    </row>
+    <row r="29" spans="1:7" ht="105">
+      <c r="A29" s="13"/>
+      <c r="B29" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C29" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="17" t="s">
+      <c r="D29" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E29" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F29" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="16">
+      <c r="G29" s="16">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="21">
-      <c r="A29" s="21" t="s">
+    <row r="30" spans="1:7" ht="21">
+      <c r="A30" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="25"/>
-    </row>
-    <row r="30" spans="1:7" ht="30">
-      <c r="A30" s="19" t="s">
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="26"/>
+    </row>
+    <row r="31" spans="1:7" ht="30">
+      <c r="A31" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B31" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="15"/>
-    </row>
-    <row r="31" spans="1:7" ht="409.5">
-      <c r="A31" s="13"/>
-      <c r="B31" s="17" t="s">
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="15"/>
+    </row>
+    <row r="32" spans="1:7" ht="409.5">
+      <c r="A32" s="13"/>
+      <c r="B32" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C32" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D32" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E32" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F32" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="16">
+      <c r="G32" s="16">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="21">
-      <c r="A32" s="21" t="s">
+    <row r="33" spans="1:7" ht="21">
+      <c r="A33" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A30:G30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2422,7 +2456,7 @@
   <dimension ref="A1:B79"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>